<commit_message>
Completed first half of schematic
</commit_message>
<xml_diff>
--- a/TimesheetWade.xlsx
+++ b/TimesheetWade.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Windows Files\Github\KiCad-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1420B91-A413-4F99-A7CB-654E7E1F81C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E209F815-EF03-4439-B8AC-4372BC3EEC94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,8 +575,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -803,7 +803,7 @@
         <v>43991</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -812,11 +812,11 @@
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="G16" s="3">
         <f>(D16-C16)+(F16-E16)</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -881,7 +881,7 @@
         <v>43994</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -890,11 +890,11 @@
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G19" s="3">
         <f>(D19-C19)+(F19-E19)</f>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -904,12 +904,9 @@
       </c>
       <c r="G21" s="7">
         <f>SUM(G15:G19)</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="8">
-        <f>SUM(G11, G21)</f>
-        <v>0.43749999999999989</v>
-      </c>
+        <v>0.22916666666666663</v>
+      </c>
+      <c r="H21" s="8"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">

</xml_diff>